<commit_message>
finished basic functions and began others
</commit_message>
<xml_diff>
--- a/scoring_lookup.xlsx
+++ b/scoring_lookup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="11475" windowHeight="7485" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="11475" windowHeight="7485" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BDItotal" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>measName</t>
   </si>
@@ -615,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,19 +648,10 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2">
-        <v>7</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -692,7 +683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finished writing core functions
</commit_message>
<xml_diff>
--- a/scoring_lookup.xlsx
+++ b/scoring_lookup.xlsx
@@ -4,29 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="11475" windowHeight="7485" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="11475" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="BDItotal" sheetId="1" r:id="rId1"/>
     <sheet name="SSQNtotal" sheetId="2" r:id="rId2"/>
     <sheet name="SSQStotal" sheetId="3" r:id="rId3"/>
+    <sheet name="HAMD6total" sheetId="4" r:id="rId4"/>
+    <sheet name="HRSD6total" sheetId="5" r:id="rId5"/>
+    <sheet name="HRSD17total" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="41">
   <si>
     <t>measName</t>
   </si>
   <si>
-    <t>forwNames</t>
-  </si>
-  <si>
-    <t>revNames</t>
-  </si>
-  <si>
     <t>revInt</t>
   </si>
   <si>
@@ -133,6 +130,18 @@
   </si>
   <si>
     <t>X6S</t>
+  </si>
+  <si>
+    <t>forwItems</t>
+  </si>
+  <si>
+    <t>revItems</t>
+  </si>
+  <si>
+    <t>HAMD6</t>
+  </si>
+  <si>
+    <t>HRSD</t>
   </si>
 </sst>
 </file>
@@ -473,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,121 +498,121 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -615,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,46 +641,46 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -684,7 +693,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,46 +706,287 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
         <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>